<commit_message>
dev: reassign ui text, Data Controller will do to Instantiate data
</commit_message>
<xml_diff>
--- a/20201010 근간 스토리.xlsx
+++ b/20201010 근간 스토리.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="130">
   <si>
     <t>전쟁이 한참이었다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -463,6 +464,86 @@
   </si>
   <si>
     <t>(아직 이해하지 못한 듯 했다.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오늘은 적당히 달리는 법을 배울 거야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>간호 안드로이드로 만들어진 제겐 이 정도가 한계네요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시속 10km 정도로 달려보겠어?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">엘림의 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공을 던져 보라고요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아, 수류탄처럼 말입니까?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아니.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가 받을 수 있도록 말이야.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>네?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박사님을 향해 수류탄, 아니 공을요?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그래, 캐치볼을 해보자고.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>엘림의 손이 부들부들 떨리더니 공이 바닥으로 툭하고 떨어졌다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인공 관절의 힘을 제대로 조정할 자신이 없습니다. 박사님.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>★ 스포츠 체험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>★ 영상 보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>괜찮아. 마음을 편하게 먹고 던져 봐.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>★ 예술 활동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">★ </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -863,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E75"/>
+  <dimension ref="A2:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1199,6 +1280,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="C53" t="s">
         <v>84</v>
       </c>
@@ -1360,6 +1444,108 @@
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B75" s="4" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B79" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B81" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B89" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B90" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>111</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B97" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B100" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B110" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>